<commit_message>
Задание 3.4.2, 3.4.3, 3.5.1
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Статистика по годам" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Статистика по городам" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Статистика по годам" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Статистика по городам" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,274 +490,342 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>2007</v>
+        <v>2003</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>38916</v>
+        <v>1366</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>41000</v>
+        <v/>
       </c>
       <c r="D2" s="2" t="n">
-        <v>2196</v>
+        <v>1983</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>2008</v>
+        <v>2004</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>43646</v>
+        <v>1488</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>49390</v>
+        <v/>
       </c>
       <c r="D3" s="2" t="n">
-        <v>17549</v>
+        <v>7833</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>2009</v>
+        <v>2005</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>42492</v>
+        <v>13331</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>40084</v>
+        <v/>
       </c>
       <c r="D4" s="2" t="n">
-        <v>17709</v>
+        <v>16022</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>2010</v>
+        <v>2006</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>43846</v>
+        <v>1522</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>47090</v>
+        <v/>
       </c>
       <c r="D5" s="2" t="n">
-        <v>29093</v>
+        <v>33321</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>84</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>2011</v>
+        <v>2007</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>47451</v>
+        <v>5604</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>52335</v>
+        <v>27500</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>36700</v>
+        <v>53562</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>134</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>2012</v>
+        <v>2008</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>48243</v>
+        <v>27478</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>51390</v>
+        <v>22000</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>44153</v>
+        <v>75070</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>110</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>2013</v>
+        <v>2009</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>51510</v>
+        <v>37548</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>54076</v>
+        <v/>
       </c>
       <c r="D8" s="2" t="n">
-        <v>59954</v>
+        <v>52889</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>137</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>2014</v>
+        <v>2010</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>50658</v>
+        <v>40958</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>56322</v>
+        <v>35000</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>66837</v>
+        <v>93494</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>155</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>2015</v>
+        <v>2011</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>52696</v>
+        <v>42359</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>44904</v>
+        <v>33666</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>70039</v>
+        <v>142458</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>256</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>62675</v>
+        <v>44540</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>47359</v>
+        <v>28800</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>75145</v>
+        <v>173897</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>285</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>60935</v>
+        <v>46218</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>45502</v>
+        <v>38050</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>82823</v>
+        <v>234019</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>447</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>58335</v>
+        <v>48482</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>46748</v>
+        <v>29681</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>131701</v>
+        <v>259571</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>620</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>69467</v>
+        <v>50654</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>60365</v>
+        <v>28653</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>115086</v>
+        <v>284763</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>435</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>73431</v>
+        <v>58261</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>66548</v>
+        <v>34538</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>102243</v>
+        <v>332460</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>364</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>82690</v>
+        <v>61724</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>69845</v>
+        <v>35071</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>57623</v>
+        <v>391464</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>167</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>65563</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>46296</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>517670</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>78212</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>51657</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>535956</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>90537</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>40704</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>489472</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>105356</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>61594</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>287915</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
         <v>2022</v>
       </c>
-      <c r="B17" s="2" t="n">
-        <v>91795</v>
-      </c>
-      <c r="C17" s="2" t="n">
-        <v>78964</v>
-      </c>
-      <c r="D17" s="2" t="n">
-        <v>18294</v>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>92</v>
+      <c r="B21" s="2" t="n">
+        <v>124935</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>47928</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>91142</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -816,57 +884,57 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
+          <t>Алматы</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>179001</v>
+      </c>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  </t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
           <t>Москва</t>
         </is>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>76970</v>
-      </c>
-      <c r="C2" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>Москва</t>
-        </is>
-      </c>
       <c r="E2" s="5" t="n">
-        <v>0.3246</v>
+        <v>0.4917</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>70218</v>
+      </c>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  </t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
           <t>Санкт-Петербург</t>
         </is>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>65286</v>
-      </c>
-      <c r="C3" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>Санкт-Петербург</t>
-        </is>
-      </c>
       <c r="E3" s="5" t="n">
-        <v>0.1197</v>
+        <v>0.1493</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Новосибирск</t>
+          <t>Санкт-Петербург</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>62254</v>
+        <v>61230</v>
       </c>
       <c r="C4" s="4" t="inlineStr">
         <is>
@@ -875,21 +943,21 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>Новосибирск</t>
+          <t>Минск</t>
         </is>
       </c>
       <c r="E4" s="5" t="n">
-        <v>0.0271</v>
+        <v>0.0598</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>Екатеринбург</t>
+          <t>Новосибирск</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>60962</v>
+        <v>57592</v>
       </c>
       <c r="C5" s="4" t="inlineStr">
         <is>
@@ -898,21 +966,21 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>Казань</t>
+          <t>Киев</t>
         </is>
       </c>
       <c r="E5" s="5" t="n">
-        <v>0.0237</v>
+        <v>0.0474</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>Казань</t>
+          <t>Екатеринбург</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>52580</v>
+        <v>54972</v>
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
@@ -921,11 +989,11 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>Нижний Новгород</t>
+          <t>Новосибирск</t>
         </is>
       </c>
       <c r="E6" s="5" t="n">
-        <v>0.0232</v>
+        <v>0.0348</v>
       </c>
     </row>
     <row r="7">
@@ -935,7 +1003,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>51644</v>
+        <v>50049</v>
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
@@ -944,21 +1012,21 @@
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>Ростов-на-Дону</t>
+          <t>Нижний Новгород</t>
         </is>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.0209</v>
+        <v>0.0316</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>Челябинск</t>
+          <t>Казань</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>51265</v>
+        <v>47800</v>
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
@@ -971,7 +1039,7 @@
         </is>
       </c>
       <c r="E8" s="5" t="n">
-        <v>0.0207</v>
+        <v>0.029</v>
       </c>
     </row>
     <row r="9">
@@ -981,7 +1049,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>50994</v>
+        <v>46337</v>
       </c>
       <c r="C9" s="4" t="inlineStr">
         <is>
@@ -990,21 +1058,21 @@
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>Краснодар</t>
+          <t>Алматы</t>
         </is>
       </c>
       <c r="E9" s="5" t="n">
-        <v>0.0185</v>
+        <v>0.0279</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>Пермь</t>
+          <t>Нижний Новгород</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>48089</v>
+        <v>44775</v>
       </c>
       <c r="C10" s="4" t="inlineStr">
         <is>
@@ -1013,21 +1081,21 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>Самара</t>
+          <t>Воронеж</t>
         </is>
       </c>
       <c r="E10" s="5" t="n">
-        <v>0.0143</v>
+        <v>0.0274</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>Нижний Новгород</t>
+          <t>Пермь</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>47662</v>
+        <v>44542</v>
       </c>
       <c r="C11" s="4" t="inlineStr">
         <is>
@@ -1036,11 +1104,11 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>Воронеж</t>
+          <t>Казань</t>
         </is>
       </c>
       <c r="E11" s="5" t="n">
-        <v>0.0141</v>
+        <v>0.0273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>